<commit_message>
Todo el modelo mat implementado, falta depurar
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\.spyder-py3\IO\casos\caso4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VICTOR\.spyder-py3\Caso 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666A31A-FE3E-427E-86A5-C088DA8614FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{D5F38296-5F6F-4A22-A382-4DFE5C3C0CDA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>12 p.m. to 6 a.m.</t>
   </si>
@@ -87,21 +86,6 @@
   </si>
   <si>
     <t>MW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 000 </t>
-  </si>
-  <si>
-    <t>27 000</t>
-  </si>
-  <si>
-    <t>40 000</t>
-  </si>
-  <si>
-    <t>25 000</t>
-  </si>
-  <si>
-    <t>15 000</t>
   </si>
   <si>
     <t>Mínima producción MW</t>
@@ -116,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,10 +371,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,24 +688,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61A1E79-2300-475F-973A-769C25B56E47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -729,78 +713,78 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="18"/>
+      <c r="C4" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D4" s="17"/>
       <c r="E4">
         <f>12-6</f>
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
+      <c r="C5" s="4">
+        <v>30000</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>20</v>
+      <c r="C6" s="4">
+        <v>25000</v>
       </c>
       <c r="E6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>19</v>
+      <c r="C7" s="4">
+        <v>40000</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
+      <c r="C8" s="4">
+        <v>27000</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
       <c r="C12" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>5</v>
@@ -812,7 +796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>8</v>
       </c>
@@ -832,7 +816,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
@@ -852,7 +836,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
@@ -872,13 +856,13 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="17" t="s">
+    <row r="18" spans="2:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>8</v>
       </c>
@@ -886,7 +870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>9</v>
       </c>
@@ -894,7 +878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="13" t="s">
         <v>10</v>
       </c>
@@ -902,13 +886,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="17" t="s">
+    <row r="23" spans="2:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="18"/>
+    </row>
+    <row r="24" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15">
         <v>0.15</v>
       </c>

</xml_diff>